<commit_message>
Update evidence for Task A7-A20, B1-B7
</commit_message>
<xml_diff>
--- a/landerosua/evidence.xlsx
+++ b/landerosua/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e6c20f8644ae710/Рабочий стол/111/noda/gameofnft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{E807ABD6-6B6A-42B1-9047-F43B7780CB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E97EA577-377E-440C-95A8-F8D79D413C8C}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{E807ABD6-6B6A-42B1-9047-F43B7780CB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06BC93C3-B651-4EA2-92B9-5D0A636D4DDA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,47 +38,27 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="27" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="88">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -164,13 +144,178 @@
   </si>
   <si>
     <t>wasm.juno1aff4yjmkp9lqce596pujxnknfthrpyj3c0n7dmm7q6rr0gz37pzsz49e9z</t>
+  </si>
+  <si>
+    <t>ibc/5585E95F90D92C12B4BE066238D26F183A669462E74AE57BAA5B4CFC576D19A6</t>
+  </si>
+  <si>
+    <t>ibc/7F871080B451C0749A4F4FBCCE131BB3D5CF8EC7EB8DE4D42CB813B9134EA2CF</t>
+  </si>
+  <si>
+    <t>ibc/ED106F85F82662C4ADAD989AD9CBA38AB16668B747D9600C4A9E68BC67B95BB0</t>
+  </si>
+  <si>
+    <t>nft7</t>
+  </si>
+  <si>
+    <t>nft8</t>
+  </si>
+  <si>
+    <t>nft9</t>
+  </si>
+  <si>
+    <t>ibc/D895BFCD5FBE6E2809850A6032C34BE9475513C7BFB1B2FB77799FDF4F916B33</t>
+  </si>
+  <si>
+    <t>nft10</t>
+  </si>
+  <si>
+    <t>nft11</t>
+  </si>
+  <si>
+    <t>nft12</t>
+  </si>
+  <si>
+    <t>ibc/AF34B0EC480C9036EDC2F79674A4E1F1A00B71EA3F88FF4AF2E2B166DAE18C03</t>
+  </si>
+  <si>
+    <t>ibc/7D614F4883094EE115E501A45B641AAE6FBCD73FC5A3D443A903E93AA498E05E</t>
+  </si>
+  <si>
+    <t>603234F0E6D23A90A18C4C27FE7F2199F65648E00455F400D5ACA107A24A7A27</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>ED88C10FC0E4AAAFC57915AE881538FC83575C10A5502D1E67D40ECFF84354F1</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>CF3A5136DECDC00F05D63BA05BA5A40E719E6DFA7B66F711B83F04455626563D</t>
+  </si>
+  <si>
+    <t>64D32ACBAB7068479ED3C72D1BBF42D49B83AE457A62F399B7E3297C67952A90</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>A6D371EE886475F2A99451C0054E9F4D15046E31DBC9553D20631A8E0A8DB834</t>
+  </si>
+  <si>
+    <t>0AE63669CA31A662B80CBF100A393C1D26A71D129E32C5228821A6DC860E3404</t>
+  </si>
+  <si>
+    <t>0B8A6E7DEC503B296AA1668AABF0143D86A3DC5F6B5208DE4878973E3B0899C7</t>
+  </si>
+  <si>
+    <t>144C5D5AC3820EAE603E71AD623BC5F95AE103DD01E4D472D0653F120F8D0616</t>
+  </si>
+  <si>
+    <t>5E53959E28074F076B91805454E3C2114A3E6E1713D3782DC62AA1B708EEA63F</t>
+  </si>
+  <si>
+    <t>3717EADECF5B8A506411FFF2AA1691796B408A868692DF63E304D6DFEF0E4C00</t>
+  </si>
+  <si>
+    <t>76E75A82761C78F68550ECA0691C8EDE57735D8641BDEB8DC0E94A8ADCDE4039</t>
+  </si>
+  <si>
+    <t>24B15AB2EDE0E039260F6B0A40727B37496D926095CB1847D6F7B62791DCF3AC</t>
+  </si>
+  <si>
+    <t>F64928AF4B541DB1E875FBEE53DE038FFEC76D1DBF3AA04E16ACDB69C3773D27</t>
+  </si>
+  <si>
+    <t>ED8EC484C8DAB502243BBC47FF3278FB4B9199E68113AB480C04AC6A7497E0D9</t>
+  </si>
+  <si>
+    <t>52D4BEFA022633F7904FEE2F64038FD9942992EF17BFBB229C4EF01B994EAF93</t>
+  </si>
+  <si>
+    <t>E4A86A9138C6C4E38854A4CFF525F076408940212ADC8ACFDF32DD22515B37F5</t>
+  </si>
+  <si>
+    <t>638E8D85E0F91BAFDB463E86969B575CFE2C53EA9C27951A6607F6E00B9247E7</t>
+  </si>
+  <si>
+    <t>CA7A49C3E60D918092433CD16E7D0BA56B91D18C7F2F9894E25B8953DC03C90D</t>
+  </si>
+  <si>
+    <t>83BE02C106F0831BF8DFC980ACDA17E43D6A600A0DE31CE068971D41F28BDE8C</t>
+  </si>
+  <si>
+    <t>726979CFECA4125CEF69C906FA5D7749ADA5C83D382596E389D6D0419176C6FA</t>
+  </si>
+  <si>
+    <t>D4BC2EE78497A77D70AE1B86AE9AB88D06D1160E4136E41A55A410166A06B4DA</t>
+  </si>
+  <si>
+    <t>395869A0BAB1FBF63E1F541FDF0A33E9B27515A0DF9F86AF4A43ED176245E2D1</t>
+  </si>
+  <si>
+    <t>F354B939DC4E7DC0B3AFFA4A80F6275FAB6AFBB21BBF9F9B96BF2ADB03E10566</t>
+  </si>
+  <si>
+    <t>FF05D24830FEE5046C52F9915E475DCE51176C6ABE8C5B4BB017C3E4EB42B8C1</t>
+  </si>
+  <si>
+    <t>58136E51A5590867032DA8F90216DB63FD54DAA0796A209091CE5DB04D0E41E6</t>
+  </si>
+  <si>
+    <t>FDF8F45C9FFF1E143DFB5A4BC15798D41E5BA13A9F9E9F0F4A363478E9A07F82</t>
+  </si>
+  <si>
+    <t>2C9AD6935C578079C9F0217632C07B4AE608525A05C21F8A50B56CF7B31AC9E1</t>
+  </si>
+  <si>
+    <t>EFB4582EB2C565898AACD4D5C1489ADA477D0EC0ECF09DE37A20CE76367A0E21</t>
+  </si>
+  <si>
+    <t>CD2B3B292ACA7B856213428C2054C15B81D3DCC3DFD8399DBC339CDBE43E2683</t>
+  </si>
+  <si>
+    <t>7178DB8BB5BD04D1738B973FF0B7ECFDC21C7681253F24A25B22868B4A783B61</t>
+  </si>
+  <si>
+    <t>9AC3BCA5F5006D11B59B25D75D626862316E4B348D8AF546F890D1082EBBEB6D</t>
+  </si>
+  <si>
+    <t>9E597F0344DA512EED979B7CD5A25F1E21E68FFB5E49A88FE578DBFB2FEB95E9</t>
+  </si>
+  <si>
+    <t>F62FBEB7EE796F79A0DD008E699A90E1E94D7A31340BA4CB603D7D99094B361F</t>
+  </si>
+  <si>
+    <t>6716D961EA1FF960819823BF11CDF7B03958DF372B08B583C9C70595AFB595B8</t>
+  </si>
+  <si>
+    <t>633A1C80C4875F8B8C8CCE3BFE27925413EE99A470F3612F2C938D7E2472D640</t>
+  </si>
+  <si>
+    <t>5397FA4E4C86C2937B05C0DDF7861DF4D0A369FB05C4E06DE392619E4BA4C409</t>
+  </si>
+  <si>
+    <t>5913FB62134BDBF332EC143F7E8FF364DD726FCDFE0041F0EB477504FDB45D0D</t>
+  </si>
+  <si>
+    <t>82B39EE19BA9A4A5B08EC78B77CE99D4D9690EDC08CE0E4DFA9FEFE220536E8A</t>
+  </si>
+  <si>
+    <t>B58CC4633AF69EFAD19B321C6DD27C0141149E7EF606BAC49218797078FD947B</t>
+  </si>
+  <si>
+    <t>2D4A63E3B32E71D80B85374E83AFBD816D7941E7778A05A4BBB94016E807F659</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +328,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -237,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -249,6 +401,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -269,6 +425,10 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -580,51 +740,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -639,7 +799,129 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -649,126 +931,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -781,13 +955,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -796,25 +972,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -827,13 +1017,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -842,25 +1034,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -875,11 +1081,13 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -888,25 +1096,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -921,11 +1135,13 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.44140625" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -934,25 +1150,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+      <c r="A2" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -965,13 +1187,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -980,25 +1204,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1011,13 +1249,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.109375" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1026,25 +1266,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1074,15 +1328,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1095,13 +1349,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1110,25 +1366,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1141,13 +1411,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1156,25 +1428,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1189,11 +1475,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1203,12 +1491,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1511,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1237,12 +1527,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1257,7 +1547,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1270,13 +1562,13 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1291,7 +1583,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1305,12 +1599,42 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CAE57C-398F-4177-A467-89E1B9395B55}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1340,32 +1664,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1396,27 +1720,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1448,27 +1772,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1499,27 +1823,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1858,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1551,66 +1875,66 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1624,28 +1948,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>